<commit_message>
example to read csv
</commit_message>
<xml_diff>
--- a/M-VT20.xlsx
+++ b/M-VT20.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="22">
   <si>
     <t xml:space="preserve">Контрольные</t>
   </si>
@@ -97,7 +97,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Helvetica Neue"/>
@@ -135,6 +135,13 @@
       <family val="1"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Helvetica Neue"/>
+      <family val="0"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -191,7 +198,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -208,10 +215,6 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -228,11 +231,19 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -261,71 +272,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H11" activeCellId="0" sqref="H11"/>
+      <selection pane="bottomRight" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="7.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="7.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="10.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="10.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="4" width="10.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="10" style="1" width="10.96"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="5" width="10.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="6.75"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="6" style="2" width="9.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="8" style="3" width="9.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="64" min="10" style="1" width="9.59"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="65" style="4" width="9.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="6" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="7" t="n">
         <v>44077</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="D2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <v>44091</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="7" t="n">
         <v>44098</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>7</v>
       </c>
     </row>
@@ -336,11 +347,28 @@
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="n">
@@ -349,17 +377,27 @@
       <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -369,11 +407,28 @@
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="11"/>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="n">
@@ -382,15 +437,27 @@
       <c r="B6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -400,21 +467,27 @@
       <c r="B7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>10</v>
+      <c r="C7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -424,21 +497,27 @@
       <c r="B8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -448,13 +527,28 @@
       <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="C9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="11"/>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="n">
@@ -463,13 +557,28 @@
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
+      <c r="C10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="n">
@@ -478,11 +587,28 @@
       <c r="B11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="n">
@@ -491,15 +617,28 @@
       <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="C12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="n">
@@ -508,11 +647,28 @@
       <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
+      <c r="C13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="n">
@@ -521,21 +677,27 @@
       <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>10</v>
+      <c r="C14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>5</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -545,42 +707,59 @@
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+      <c r="C15" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="12"/>
+      <c r="A16" s="13"/>
       <c r="C16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="C17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="12"/>
+      <c r="A18" s="13"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="C19" s="3"/>
     </row>
     <row r="20" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
+      <c r="A20" s="13"/>
       <c r="C20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="C21" s="3"/>
     </row>
     <row r="22" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
+      <c r="A22" s="13"/>
       <c r="C22" s="3"/>
     </row>
     <row r="23" customFormat="false" ht="20.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="C23" s="3"/>
     </row>
   </sheetData>

</xml_diff>